<commit_message>
cake shop db build.
</commit_message>
<xml_diff>
--- a/application/cake-shop/cakeshop-database-specification.xlsx
+++ b/application/cake-shop/cakeshop-database-specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-diya\Repo\LucasNote\application\cake-shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258D79C9-C7EC-4E3C-BCF3-C71EE8553630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E361DD5-BDEA-4A85-995F-E9EBB6BECA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ManamgementSystem" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="118">
   <si>
     <t>Field</t>
   </si>
@@ -380,6 +380,12 @@
   </si>
   <si>
     <t>CustomerDelivery</t>
+  </si>
+  <si>
+    <t>DeliveryPhoneNumber</t>
+  </si>
+  <si>
+    <t>配送电话</t>
   </si>
 </sst>
 </file>
@@ -425,13 +431,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,14 +733,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -889,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA830E8C-0807-4C41-BAEB-4E6681F66675}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -903,14 +909,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1053,14 +1059,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1203,14 +1209,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1323,23 +1329,23 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="D32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1378,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1352B1F5-9745-4365-B80B-D729E8A840D3}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,14 +1400,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1523,23 +1529,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1564,14 +1570,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1714,14 +1720,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1904,14 +1910,14 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -2047,9 +2053,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2196F9D8-747D-42DD-AD91-23C4CBEF1BC8}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2061,14 +2067,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2212,19 +2218,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -2232,13 +2238,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -2252,13 +2258,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -2272,13 +2278,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -2292,83 +2298,83 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -2382,19 +2388,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
         <v>16</v>
@@ -2402,44 +2408,44 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -2453,19 +2459,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -2473,13 +2479,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -2493,28 +2499,48 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>64</v>
       </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>